<commit_message>
work on tenant dashboard
</commit_message>
<xml_diff>
--- a/seeds/schemas/tenant.xlsx
+++ b/seeds/schemas/tenant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="418">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -769,25 +769,52 @@
     <t xml:space="preserve">partial_type_name</t>
   </si>
   <si>
+    <t xml:space="preserve">partial_type_icon</t>
+  </si>
+  <si>
     <t xml:space="preserve">home service</t>
   </si>
   <si>
+    <t xml:space="preserve">service-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">logo</t>
   </si>
   <si>
+    <t xml:space="preserve">award-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">hotel</t>
   </si>
   <si>
+    <t xml:space="preserve">hotel-bed-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">team member</t>
   </si>
   <si>
+    <t xml:space="preserve">team-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">service</t>
   </si>
   <si>
+    <t xml:space="preserve">settings-3-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">project</t>
   </si>
   <si>
+    <t xml:space="preserve">briefcase-line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gallery-line</t>
+  </si>
+  <si>
     <t xml:space="preserve">banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slideshow-line</t>
   </si>
   <si>
     <t xml:space="preserve">partial_name</t>
@@ -1472,10 +1499,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1494,6 +1517,10 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2544,15 +2571,14 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="234.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="234.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="234.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="89.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="66.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2597,7 +2623,7 @@
       <c r="A2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2606,10 +2632,10 @@
       <c r="D2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -2635,10 +2661,10 @@
       <c r="A3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>175</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -2647,10 +2673,10 @@
       <c r="E3" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>178</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -2673,10 +2699,10 @@
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>124</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2685,7 +2711,7 @@
       <c r="E4" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -2711,10 +2737,10 @@
       <c r="A5" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>182</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2723,7 +2749,7 @@
       <c r="E5" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -2749,25 +2775,25 @@
       <c r="A6" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>188</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>189</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -2787,7 +2813,7 @@
       <c r="A7" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2799,7 +2825,7 @@
       <c r="E7" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -2825,10 +2851,10 @@
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>124</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2837,7 +2863,7 @@
       <c r="E8" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -2863,10 +2889,10 @@
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>194</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -2875,7 +2901,7 @@
       <c r="E9" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -2901,10 +2927,10 @@
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2913,7 +2939,7 @@
       <c r="E10" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -2939,10 +2965,10 @@
       <c r="A11" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>143</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -2951,7 +2977,7 @@
       <c r="E11" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -2977,7 +3003,7 @@
       <c r="A12" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -3015,7 +3041,7 @@
       <c r="A13" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -3053,7 +3079,7 @@
       <c r="A14" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>210</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3091,7 +3117,7 @@
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -3129,7 +3155,7 @@
       <c r="A16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>222</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -3167,7 +3193,7 @@
       <c r="A17" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>225</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -3205,7 +3231,7 @@
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>230</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -3243,7 +3269,7 @@
       <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="3" t="s">
         <v>235</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -3281,7 +3307,7 @@
       <c r="A20" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3" t="s">
         <v>240</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -3319,7 +3345,7 @@
       <c r="A21" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -3466,14 +3492,14 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.33"/>
@@ -3486,60 +3512,81 @@
       <c r="A1" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="4"/>
+        <v>248</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>249</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>250</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>251</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>252</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>253</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>254</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>255</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B6" s="4"/>
+        <v>256</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>257</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>258</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>259</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="B8" s="13" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3560,7 +3607,7 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -3575,10 +3622,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>255</v>
+        <v>263</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>18</v>
@@ -3587,63 +3634,63 @@
         <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>267</v>
+        <v>275</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>276</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>181</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>268</v>
+        <v>252</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>277</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>168</v>
@@ -3663,31 +3710,31 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>272</v>
+        <v>280</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>181</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>273</v>
+        <v>252</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>282</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>168</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>168</v>
@@ -3707,31 +3754,31 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>277</v>
+        <v>285</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>181</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>278</v>
+        <v>252</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>287</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>168</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>168</v>
@@ -3751,25 +3798,25 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>280</v>
+        <v>288</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>289</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>181</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>281</v>
+        <v>252</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>290</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>282</v>
+      <c r="G5" s="12" t="s">
+        <v>291</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>168</v>
@@ -3795,25 +3842,25 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="C6" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>285</v>
+        <v>248</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>294</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>286</v>
+      <c r="G6" s="12" t="s">
+        <v>295</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>168</v>
@@ -3839,25 +3886,25 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F7" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>168</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>168</v>
@@ -3882,26 +3929,26 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="F8" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>168</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>168</v>
@@ -3927,25 +3974,25 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>295</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="C9" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>298</v>
+        <v>248</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>168</v>
@@ -3971,130 +4018,130 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>300</v>
+        <v>308</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>301</v>
+        <v>258</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>310</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>168</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>168</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>304</v>
+        <v>279</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>313</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>307</v>
+      <c r="A11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>316</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>273</v>
+        <v>258</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>282</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>168</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>168</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>310</v>
+        <v>284</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>312</v>
+        <v>285</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>313</v>
+        <v>258</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>322</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>168</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L12" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="M12" s="13" t="s">
+      <c r="L12" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" s="12" t="s">
         <v>168</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -4103,42 +4150,42 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>315</v>
+        <v>288</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>324</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>316</v>
+        <v>258</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>325</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>168</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L13" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="M13" s="13" t="s">
+      <c r="L13" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="12" t="s">
         <v>168</v>
       </c>
       <c r="N13" s="6" t="s">
@@ -4147,28 +4194,28 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>319</v>
+        <v>327</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>320</v>
+        <v>258</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>329</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>168</v>
@@ -4190,29 +4237,29 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>323</v>
+      <c r="A15" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>332</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>320</v>
+        <v>258</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>329</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>168</v>
@@ -4235,25 +4282,25 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>325</v>
+        <v>333</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>334</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="G16" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>168</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>168</v>
@@ -4276,19 +4323,19 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>328</v>
+        <v>336</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>337</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>168</v>
@@ -4297,7 +4344,7 @@
         <v>168</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>168</v>
@@ -4319,20 +4366,20 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>332</v>
+      <c r="A18" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>341</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>293</v>
+        <v>256</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>168</v>
@@ -4341,13 +4388,13 @@
         <v>168</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>168</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>168</v>
@@ -4364,19 +4411,19 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>335</v>
+        <v>343</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>168</v>
@@ -4385,7 +4432,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>168</v>
@@ -4408,19 +4455,19 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>338</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>339</v>
+        <v>347</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>348</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>168</v>
@@ -4429,19 +4476,19 @@
         <v>168</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>168</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>168</v>
@@ -4452,19 +4499,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>344</v>
+        <v>352</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>353</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>168</v>
@@ -4473,7 +4520,7 @@
         <v>168</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>168</v>
@@ -4496,28 +4543,28 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>348</v>
+        <v>356</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>168</v>
@@ -4540,28 +4587,28 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>353</v>
+        <v>361</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>362</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>168</v>
@@ -4584,28 +4631,28 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>358</v>
+        <v>366</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>367</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="F24" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>168</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>168</v>
@@ -4628,28 +4675,28 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>362</v>
+        <v>370</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>371</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>168</v>
@@ -4671,29 +4718,29 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>366</v>
+      <c r="A26" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>375</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>168</v>
@@ -4715,310 +4762,310 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="A27" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J27" s="8" t="s">
+      <c r="D27" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N27" s="8" t="s">
+      <c r="K27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N27" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="A28" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" s="8" t="s">
+      <c r="D28" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="K28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N28" s="8" t="s">
+      <c r="K28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N28" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="A29" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>386</v>
+      <c r="D29" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="A30" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>392</v>
+      <c r="D30" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="A31" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>398</v>
+      <c r="D31" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="A32" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N32" s="8" t="s">
+      <c r="D32" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N32" s="3" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="A33" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="N33" s="8" t="s">
+      <c r="D33" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N33" s="3" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>